<commit_message>
Scrape Global => consolidated_data
</commit_message>
<xml_diff>
--- a/data/adm/adm_tenders.xlsx
+++ b/data/adm/adm_tenders.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>objet</t>
   </si>
@@ -22,32 +22,19 @@
     <t>date_limite</t>
   </si>
   <si>
-    <t>Objet
-                                                        : 
-                                                    La réalisation des travaux d’entretien de la chaussée des autoroutes Kenitra – Sidi El Yamani et Khémisset – Meknes « PROGRAMME 2025-2026 »</t>
-  </si>
-  <si>
-    <t>Objet
-                                                        : 
-                                                    La réalisation des travaux d’entretien des Bâtiments des axes autoroutiers Nord, Centre et Est</t>
-  </si>
-  <si>
-    <t>Objet
-                                                        : 
-                                                     La réalisation des travaux de construction des viaducs sur Oued Cherrat et sur Oued Yquem de l'autoroute Rabat Casablanca Continentale</t>
-  </si>
-  <si>
-    <t>Objet
-                                                        : 
-                                                    Mise en conformité de la ligne 60 kV N°107-1 MOHAMMEDIA-ONCF EL MANSOURIA nécessitée par le projet d’aménagement des Routes Provinciales N°3304 et N°3308 pour la desserte du futur Grand Stade HASSAN II - Province</t>
-  </si>
-  <si>
-    <t>Objet
-                                                        : 
-                                                     La réalisation des prestations de transport du personnel d’ADM</t>
-  </si>
-  <si>
-    <t>Date limite de remise des plis</t>
+    <t>La réalisation des travaux d’entretien de la chaussée des autoroutes Kenitra – Sidi El Yamani et Khémisset – Meknes « PROGRAMME 2025-2026 »</t>
+  </si>
+  <si>
+    <t>La réalisation des travaux d’entretien des Bâtiments des axes autoroutiers Nord, Centre et Est</t>
+  </si>
+  <si>
+    <t>La réalisation des travaux de construction des viaducs sur Oued Cherrat et sur Oued Yquem de l'autoroute Rabat Casablanca Continentale</t>
+  </si>
+  <si>
+    <t>Mise en conformité de la ligne 60 kV N°107-1 MOHAMMEDIA-ONCF EL MANSOURIA nécessitée par le projet d’aménagement des Routes Provinciales N°3304 et N°3308 pour la desserte du futur Grand Stade HASSAN II - Province</t>
+  </si>
+  <si>
+    <t>La réalisation des prestations de transport du personnel d’ADM</t>
   </si>
   <si>
     <t>N/A</t>
@@ -408,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -432,15 +419,15 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -448,58 +435,18 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scraper data + show data MVC
</commit_message>
<xml_diff>
--- a/data/adm/adm_tenders.xlsx
+++ b/data/adm/adm_tenders.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>objet</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>La réalisation des travaux d’entretien de la chaussée des autoroutes Kenitra – Sidi El Yamani et Khémisset – Meknes « PROGRAMME 2025-2026 »</t>
+  </si>
+  <si>
+    <t>Mise en Conformité des lignes électriques HTA et BT interceptés par le projet de l’autoroute Rabat-Casablanca Continentale</t>
   </si>
   <si>
     <t>La réalisation des travaux d’entretien des Bâtiments des axes autoroutiers Nord, Centre et Est</t>
@@ -395,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,7 +417,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -422,7 +425,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -430,7 +433,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -438,7 +441,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -446,7 +449,15 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
scraping + template - amelioration
</commit_message>
<xml_diff>
--- a/data/adm/adm_tenders.xlsx
+++ b/data/adm/adm_tenders.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>objet</t>
   </si>
@@ -43,13 +43,25 @@
     <t>La réalisation des travaux de construction des viaducs sur Oued Cherrat et sur Oued Yquem de l'autoroute Rabat Casablanca Continentale</t>
   </si>
   <si>
-    <t>Mise en conformité de la ligne 60 kV N°107-1 MOHAMMEDIA-ONCF EL MANSOURIA nécessitée par le projet d’aménagement des Routes Provinciales N°3304 et N°3308 pour la desserte du futur Grand Stade HASSAN II - Province</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
     <t>https://achats.adm.co.ma/?page=entreprise.EntrepriseDetailsConsultation&amp;refConsultation=4410&amp;orgAcronyme=e3r&amp;echanges</t>
+  </si>
+  <si>
+    <t>https://achats.adm.co.ma/?page=entreprise.EntrepriseDetailsConsultation&amp;refConsultation=4409&amp;orgAcronyme=e3r&amp;echanges</t>
+  </si>
+  <si>
+    <t>https://achats.adm.co.ma/?page=entreprise.EntrepriseDetailsConsultation&amp;refConsultation=4387&amp;orgAcronyme=e3r&amp;echanges</t>
+  </si>
+  <si>
+    <t>https://achats.adm.co.ma/?page=entreprise.EntrepriseDetailsConsultation&amp;refConsultation=4408&amp;orgAcronyme=e3r&amp;echanges</t>
+  </si>
+  <si>
+    <t>https://achats.adm.co.ma/?page=entreprise.EntrepriseDetailsConsultation&amp;refConsultation=4403&amp;orgAcronyme=e3r&amp;echanges</t>
+  </si>
+  <si>
+    <t>https://achats.adm.co.ma/?page=entreprise.EntrepriseDetailsConsultation&amp;refConsultation=4386&amp;orgAcronyme=e3r&amp;echanges</t>
   </si>
 </sst>
 </file>
@@ -420,7 +432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -442,10 +454,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -453,7 +465,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
@@ -464,10 +476,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -475,10 +487,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -486,10 +498,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -497,21 +509,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -522,7 +523,6 @@
     <hyperlink ref="C5" r:id="rId4"/>
     <hyperlink ref="C6" r:id="rId5"/>
     <hyperlink ref="C7" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>